<commit_message>
First test showing that phi.u is NA.
</commit_message>
<xml_diff>
--- a/inst/extdata/Machines - Data/Airplanes/Airplanes.xlsx
+++ b/inst/extdata/Machines - Data/Airplanes/Airplanes.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B214A906-4CC8-B74A-B217-07F48A4B6E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -97,7 +98,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,7 +186,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2 3" xfId="1"/>
+    <cellStyle name="Normal 2 2 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -462,21 +463,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="3" max="3" width="54.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="3" max="3" width="54.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -487,7 +488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -498,7 +499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -513,24 +514,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -539,7 +540,7 @@
       <c r="D1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -568,7 +569,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -597,7 +598,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -626,56 +627,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="17" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="19" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="20" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -899,18 +900,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -933,14 +934,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D57BA165-9822-445B-B328-4F06AD982831}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF083C1D-CE62-48EF-BAF9-9D27C80F6E5E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="83e0870f-5ab0-41af-b2c4-f358cb535498"/>
@@ -955,4 +948,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D57BA165-9822-445B-B328-4F06AD982831}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>